<commit_message>
Addition and minor fixes
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/Rev 2.0/BOM-speeduino v0.4.3 compatible PCB for m40 rev2.0.xlsx
+++ b/m50,m40,m60 Pnp/Rev 2.0/BOM-speeduino v0.4.3 compatible PCB for m40 rev2.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A945DEA1-FFEB-4598-8AF5-3C0240C9E5EA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A83D82-320D-4455-AE78-8F3FA8D39117}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="2805" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -2036,7 +2036,7 @@
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3335,7 +3335,7 @@
     </row>
     <row r="24" spans="1:19" ht="16.5" thickBot="1">
       <c r="A24" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>200</v>
@@ -3368,28 +3368,28 @@
       </c>
       <c r="M24" s="6">
         <f>K24*A24</f>
-        <v>0.23</v>
+        <v>0.46</v>
       </c>
       <c r="N24" s="6">
         <f>L24*A24</f>
-        <v>0.49</v>
+        <v>0.98</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>1,SAM1213-02-ND</v>
+        <v>2,SAM1213-02-ND</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="7"/>
-        <v>1x 2 POS Header</v>
+        <v>2x 2 POS Header</v>
       </c>
       <c r="R24" t="str">
         <f t="shared" si="4"/>
-        <v>200-SSW10201TS|1</v>
+        <v>200-SSW10201TS|2</v>
       </c>
       <c r="S24" t="str">
         <f t="shared" si="5"/>
-        <v>SSW-102-01-T-S 1</v>
+        <v>SSW-102-01-T-S 2</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="16.5" thickBot="1">
@@ -5095,11 +5095,11 @@
       <c r="L58" s="1"/>
       <c r="M58" s="10">
         <f>SUM(M3:M53)</f>
-        <v>77.420000000000016</v>
+        <v>77.650000000000006</v>
       </c>
       <c r="N58" s="10">
         <f>SUM(N3:N53)</f>
-        <v>96.472000000000023</v>
+        <v>96.962000000000018</v>
       </c>
       <c r="O58" s="9" t="s">
         <v>65</v>

</xml_diff>